<commit_message>
Update Lazada and lazada data processing
</commit_message>
<xml_diff>
--- a/Data/Products_Lazada.xlsx
+++ b/Data/Products_Lazada.xlsx
@@ -19,6 +19,9 @@
     <x:sheet name="shirts-for-men" sheetId="7" r:id="rId7"/>
     <x:sheet name="dress-for-women" sheetId="8" r:id="rId8"/>
     <x:sheet name="bag-for-women" sheetId="9" r:id="rId9"/>
+    <x:sheet name="shoes" sheetId="10" r:id="rId10"/>
+    <x:sheet name="bags" sheetId="11" r:id="rId11"/>
+    <x:sheet name="accessories" sheetId="12" r:id="rId12"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="0"/>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="903">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="1254">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -2735,6 +2738,1059 @@
   </x:si>
   <x:si>
     <x:t>197 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>384 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025 New Korean Style Women's Shoes Fashion Sneakers Breathable Soft Sole Running Shoes Ladies Casual Shoes Cross-border</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/2025-new-korean-style-womens-shoes-fashion-sneakers-breathable-soft-sole-running-shoes-ladies-casual-shoes-cross-border-i3422192944.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4.43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>White Shoes Women's 2023 Spring New Versatile Platform Shoes Korean Style for Children and Students ins Harajuku Style Sneakers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/white-shoes-womens-2023-spring-new-versatile-platform-shoes-korean-style-for-children-and-students-ins-harajuku-style-sneakers-i2630087088.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$6.38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 78%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New 2024 Spring Women's Sneakers Lightweight Sport Shoes with Thick Sole and Internal Heel Increase for a Slimming Leg Effect Casual Style Rubber Outsole and Mesh Interior</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/new-2024-spring-womens-sneakers-lightweight-sport-shoes-with-thick-sole-and-internal-heel-increase-for-a-slimming-leg-effect-casual-style-rubber-outsole-and-mesh-interior-i3109155636.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$9.85</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.1K sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2023 New Fashionable Cotton-Padded Shoes for Women Autumn and Winter Women's Shoes Fleece-Lined Sneakers High-Top Women's Shoes for Students Korean Style Clunky Sneakers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/2023-new-fashionable-cotton-padded-shoes-for-women-autumn-and-winter-womens-shoes-fleece-lined-sneakers-high-top-womens-shoes-for-students-korean-style-clunky-sneakers-i2898874651.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$8.86</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 63%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>174 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>women shoes Women's scholl shoes scholl ladies shoes woman Kasut wanita Scholl Ladies Casual Shoe Kamila - DL6691 Women Sneakers Women Boat Shoes &amp; Loafers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/women-shoes-womens-scholl-shoes-scholl-ladies-shoes-woman-kasut-wanita-scholl-ladies-casual-shoe-kamila-dl6691-women-sneakers-women-boat-shoes-loafers-i2695332100.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$12.06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>207 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>scholl women shoes scholl ladies shoes Scholl Women's Casual Shoes Scholl Sneakers Women Boat Shoes Kasut wanita women shoes sport Sneakers Lifestyle Casual shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/scholl-women-shoes-scholl-ladies-shoes-scholl-womens-casual-shoes-scholl-sneakers-women-boat-shoes-kasut-wanita-women-shoes-sport-sneakers-lifestyle-casual-shoes-i2931001734.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$10.95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ewtry Women's Casual Sneakers Glitter Squins Low Top Lace Up Platform Sneakers for Women Ladies and Teen Girls EWT-MY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/ewtry-womens-casual-sneakers-glitter-squins-low-top-lace-up-platform-sneakers-for-women-ladies-and-teen-girls-ewt-my-i3038939634.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$14.74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/women-shoes-womens-scholl-shoes-scholl-ladies-shoes-woman-kasut-wanita-scholl-ladies-casual-shoe-kamila-dl6691-women-sneakers-women-boat-shoes-loafers-i2695098970.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 72%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>58 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Eircan Casual Women's Shoes Breathable Running Shoes Retro Low Top Sneakers Comfortable Spring Autumn Summer Seasonal Footwear</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/eircan-casual-womens-shoes-breathable-running-shoes-retro-low-top-sneakers-comfortable-spring-autumn-summer-seasonal-footwear-i3173304901.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$8.33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zhao Lusi Maillard Baseball Star Captain Dad Shoes Women's Korean Style Retro Easy Matching Mesh Casual Sneaker</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/zhao-lusi-maillard-baseball-star-captain-dad-shoes-womens-korean-style-retro-easy-matching-mesh-casual-sneaker-i3275244394.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LOMOGI Superme Women Sneaker Shoes Sport kasut perempuan Running Shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/lomogi-superme-women-sneaker-shoes-sport-kasut-perempuan-running-shoes-i2787501656.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4.06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full Black Leather Surface Waterproof Sport Shoes Comfortable Soft Bottom Work Shoes for Women Anti-Slip Kitchen Shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/full-black-leather-surface-waterproof-sport-shoes-comfortable-soft-bottom-work-shoes-for-women-anti-slip-kitchen-shoes-i3420211477.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2.56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DOSREAL Hot Sale Dance Shoes For Woman Practice Shoes Modern Dance Jazz Shoes Sneakers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/dosreal-hot-sale-dance-shoes-for-woman-practice-shoes-modern-dance-jazz-shoes-sneakers-i320798496.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$14.55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 58%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Women's Sport Shoes Breathable Mesh Flat Bottom Lightweight Running Travel Sneakers Spring Summer New Style MISS Seacy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/womens-sport-shoes-breathable-mesh-flat-bottom-lightweight-running-travel-sneakers-spring-summer-new-style-miss-seacy-i3415807400.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Design Heart Angel Bear with Wings Thick Bottom Dad Sneakers Casual Sport Shoes round Toe Mesh Inner Lining Synthetic Leather</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/original-design-heart-angel-bear-with-wings-thick-bottom-dad-sneakers-casual-sport-shoes-round-toe-mesh-inner-lining-synthetic-leather-i3282208890.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$9.51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Casual White Sneakers Women's Spring Autumn Youth Fashion Work Student Sports Flat Shoes Korean Style round Toe Low Heel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/casual-white-sneakers-womens-spring-autumn-youth-fashion-work-student-sports-flat-shoes-korean-style-round-toe-low-heel-i3174351716.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4.20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 New Arrival Pitaya Girl Pink Bread Shoes Student Shoes Casual Versatile Sneakers Breathable Trendy Sneaker</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/2024-new-arrival-pitaya-girl-pink-bread-shoes-student-shoes-casual-versatile-sneakers-breathable-trendy-sneaker-i3096889373.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>264 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New Old Beijing Cloth Shoes Women's Flat Bottom Breathable Summer Casual Shoes Embroidered Slip-On round Toe Rubber Outsole</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/new-old-beijing-cloth-shoes-womens-flat-bottom-breathable-summer-casual-shoes-embroidered-slip-on-round-toe-rubber-outsole-i3341336347.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$3.58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>175 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Da Dong Fang Thick Bottom Dad Shoes Women's Sporty Casual Sneakers Elementary School Students Show Feet Versatile Fall New Style</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/da-dong-fang-thick-bottom-dad-shoes-womens-sporty-casual-sneakers-elementary-school-students-show-feet-versatile-fall-new-style-i3340122377.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$5.46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>666 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Student Moral Training Shoes Female White Shoes 2024 Autumn New Arrival Minority All-Match Milk Fufu Light Pink Casual Board Shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/student-moral-training-shoes-female-white-shoes-2024-autumn-new-arrival-minority-all-match-milk-fufu-light-pink-casual-board-shoes-i3214144396.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4.29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>474 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Spring Autumn Women's Slip-On Breathable Anti-Slip Comfortable Soft Bottom Leisure Shoes Chinese Style Flat Heel round Toe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/spring-autumn-womens-slip-on-breathable-anti-slip-comfortable-soft-bottom-leisure-shoes-chinese-style-flat-heel-round-toe-i3388784476.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$7.18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>607 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sneakers Women Platform Shoes Women Sport Running Shoes Thick Bottom Ladies Wedges Running Outdoor Krasovki Women Sneakers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sneakers-women-platform-shoes-women-sport-running-shoes-thick-bottom-ladies-wedges-running-outdoor-krasovki-women-sneakers-i308632031.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$8.01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>158 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Silver Color Breathable Women's Casual Sport Shoes Thick Bottom Slip-On Versatile Comfortable round Toe Rubber Outsole Shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/silver-color-breathable-womens-casual-sport-shoes-thick-bottom-slip-on-versatile-comfortable-round-toe-rubber-outsole-shoes-i3275239801.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$5.74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>White Shoes Women's Shoes Leather Surface 2023 New Autumn and Summer Easiest for Match Casual Show Feet Small Sneaker Flats Internet-Famous Skateboard Shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/white-shoes-womens-shoes-leather-surface-2023-new-autumn-and-summer-easiest-for-match-casual-show-feet-small-sneaker-flats-internet-famous-skateboard-shoes-i3172445326.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4.86</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Old Beijing Cloth Shoes Women's Official Flagship Store New Arrival Soft Bottom Work Shoes Parka Summer Mothers' Black Gommino</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/old-beijing-cloth-shoes-womens-official-flagship-store-new-arrival-soft-bottom-work-shoes-parka-summer-mothers-black-gommino-i3102819599.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$7.94</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4.18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>444 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HuaFuAgan Women's 2024 Retro German Training Shoes Real Leather Casual Sports Flat Shoes With Cross Strap and Deep Mouth Opening</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/huafuagan-womens-2024-retro-german-training-shoes-real-leather-casual-sports-flat-shoes-with-cross-strap-and-deep-mouth-opening-i3128818114.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>601 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sneakers for Women Small White Shoes Spring and Autumn New Leisure Sports Flat Shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sneakers-for-women-small-white-shoes-spring-and-autumn-new-leisure-sports-flat-shoes-i3206612458.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$9.34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $0.47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Casual Women's Dad Shoes High Aesthetic Value Versatile Ins Trend 2023 Spring Autumn New Arrival Lightweight Sports Shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/casual-womens-dad-shoes-high-aesthetic-value-versatile-ins-trend-2023-spring-autumn-new-arrival-lightweight-sports-shoes-i3060057502.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$8.53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5.0K sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shallow Mouth Small Fragrance Style Women's Shoes Beijjing Old Style Slip-On Flat Bottom Casual Fabric Shoes Mom Shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/shallow-mouth-small-fragrance-style-womens-shoes-beijjing-old-style-slip-on-flat-bottom-casual-fabric-shoes-mom-shoes-i3388830226.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Black Canvas Shoes Unisex Breathable Lightweight Anti-slip Wear-resistant Supportive Absorbent Shockproof Low Top Rubber Outsole</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/black-canvas-shoes-unisex-breathable-lightweight-anti-slip-wear-resistant-supportive-absorbent-shockproof-low-top-rubber-outsole-i2038024099.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4.67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>324 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New Anti-Slip Soft Bottom Mom Shoes Comfortable Slip-On Women's Mesh Uppers Breathable Beijing Cloth Shoes Casual Flat Heel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/new-anti-slip-soft-bottom-mom-shoes-comfortable-slip-on-womens-mesh-uppers-breathable-beijing-cloth-shoes-casual-flat-heel-i3388660853.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hy908 New Casual Board Shoes 2025 Autumn Fashion Breathable Shoes Raise the Bottom Student Mid-Top Korean Fashion</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/hy908-new-casual-board-shoes-2025-autumn-fashion-breathable-shoes-raise-the-bottom-student-mid-top-korean-fashion-i3393578293.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$9.70</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 77%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LZD 102Scholl Ladies Casual Shoe Kamila Sneaker - LC1268</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/lzd-102scholl-ladies-casual-shoe-kamila-sneaker-lc1268-i3126409461.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$14.19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 23%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men's sports shoes. New high-top sneakers for 2023 summer. Fashion casual shoes. Breathable and fashionable men's flat shoes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/mens-sports-shoes-new-high-top-sneakers-for-2023-summer-fashion-casual-shoes-breathable-and-fashionable-mens-flat-shoes-i2693254077.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$6.40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LouisWill Men's Backpacks backpack for men Bag Men Laptop Backpack Waterproof Travel Backpack Business Bag College Backpack Casual Shoulder Bag Anti Theft Back Pack School Bag for Men Women back pack bag for men</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/louiswill-mens-backpacks-backpack-for-men-bag-men-laptop-backpack-waterproof-travel-backpack-business-bag-college-backpack-casual-shoulder-bag-anti-theft-back-pack-school-bag-for-men-women-back-pack-bag-for-men-i2447873778.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$12.21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[SG Ready Stocks] 10L /15L 20L/30L Ocean Pack Dry Bag Travel Fishing Holiday Usage Multipurpose Usage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sg-ready-stocks-10l-15l-20l30l-ocean-pack-dry-bag-travel-fishing-holiday-usage-multipurpose-usage-i1673969275.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$5.50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 21%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.5K sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Foldable Shopping Bag/Recycle Eco Bag/Shopping Bag Customization</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/foldable-shopping-bagrecycle-eco-bagshopping-bag-customization-i3115562820.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>575 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>50L Capacity Men Army Military Tactical Large Backpack Waterproof Outdoor Sport Hiking Camping Hunting 3D Rucksack Bags For Men army backpack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/50l-capacity-men-army-military-tactical-large-backpack-waterproof-outdoor-sport-hiking-camping-hunting-3d-rucksack-bags-for-men-army-backpack-i2501183037.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$13.77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 65%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Waterproof Dry Bag Backpack Professional Ocean Pack Large size hiking Diving Bag Travel Outdoor Sling Shoulder</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/waterproof-dry-bag-backpack-professional-ocean-pack-large-size-hiking-diving-bag-travel-outdoor-sling-shoulder-i2955288906.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>212 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>104 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>QIYUE Tote Bag for Women, Lightweight Puffy Duffel Bag with Compartments, Quilted Shoulder Bag Handbag for Travel, Work，Gym</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/qiyue-tote-bag-for-women-lightweight-puffy-duffel-bag-with-compartments-quilted-shoulder-bag-handbag-for-travel-workgym-i3414986402.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$9.92</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Early Bird Saved $25.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 New Commuter Large Capacity Women's Bag Striped Canvas Shoulder Crossbody Handbag Tote Bag Single Shoulder Storage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/2024-new-commuter-large-capacity-womens-bag-striped-canvas-shoulder-crossbody-handbag-tote-bag-single-shoulder-storage-i3378366212.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>434 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$6.20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>470 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tomvorks Mesh Drawstring Storage Sack Portable Camping Gear Bag Lightweight Bag for Camping Hiking Traveling with Nylon Material (S Blue)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/tomvorks-mesh-drawstring-storage-sack-portable-camping-gear-bag-lightweight-bag-for-camping-hiking-traveling-with-nylon-material-s-blue-i3409496276.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$3.40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 31%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>【FREE Noodle Gift Set Worth $19.90】Cai Lin Ji Limited Edition Tote Bag (2 Designs, 38x34cm, Eco Canvas)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/free-noodle-gift-set-worth-1990cai-lin-ji-limited-edition-tote-bag-2-designs-38x34cm-eco-canvas-i3428069925.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$9.50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>✨_xD83D__xDC96_ WHOLESALE ✨_xD83D__xDC96_♻️ (LARGE) FOLDABLE RECYCLE BAG l Tote Bag l Shopping Bag l Reusable ECO Bag l Children Day Gifts l Teachers Day Gift l Teacher Bag ✨ Hello Kitty Elmo Melody Stella Bunny Summiko Tokidoki Gudetama l Carrier</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/wholesale-large-foldable-recycle-bag-l-tote-bag-l-shopping-bag-l-reusable-eco-bag-l-children-day-gifts-l-teachers-day-gift-l-teacher-bag-hello-kitty-elmo-melody-stella-bunny-summiko-tokidoki-gudetama-l-carrier-i2892593982.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2.80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>504 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>❤️Foldable Recycle Bag❤️Eco-Friendly Shopping bag❤️SG Seller❤️ Groceries Bag Children day gift</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/foldable-recycle-bageco-friendly-shopping-bagsg-seller-groceries-bag-children-day-gift-i1629866259.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.0K sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[SG Local] Knit bag/ Lunch bag/ Shopping Bag / Portable Small Eco Bag / Tote Bag Women Handbags Gift</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sg-local-knit-bag-lunch-bag-shopping-bag-portable-small-eco-bag-tote-bag-women-handbags-gift-i3368556038.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2.45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SGFOMO Foldable Backpack Ultralight 20L Cycling Hiking Backpacks Folding Bag Daypack Small Travel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sgfomo-foldable-backpack-ultralight-20l-cycling-hiking-backpacks-folding-bag-daypack-small-travel-i3127081033.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T2P NO MOQ Packable Backpack Bag Foldable Hiking Daypack Ultralight Collapsible Water Resistant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/t2p-no-moq-packable-backpack-bag-foldable-hiking-daypack-ultralight-collapsible-water-resistant-i2962377640.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>❤️[Local Seller] shopping bag / grocery bag / storage bag / tote bag/recycle bag tote handbag /Trendy, Chic, Instagrammable eco friendly large and small capacity waterproof, foldable woven reusable shopping bag / grocery bag / storage bag / tote handbag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/local-seller-shopping-bag-grocery-bag-storage-bag-tote-bagrecycle-bag-tote-handbag-trendy-chic-instagrammable-eco-friendly-large-and-small-capacity-waterproof-foldable-woven-reusable-shopping-bag-grocery-bag-storage-bag-tote-handbag-i2110923807.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2.89</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 49%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[SG SELLER]Giant Duffel Bag For Travel Storage Sports Durable Water Resistant house moving delivery all can [179] [221]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sg-sellergiant-duffel-bag-for-travel-storage-sports-durable-water-resistant-house-moving-delivery-all-can-179-221-i2447517599.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>105 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tote Bags Woven CanvasTote Bag | LITTLE MISS DESIGNS | Custom Gifts Personalised Children Tote Bags Custom Bag for Children Birthday Gifts Pets Bag | MR MEN TOTE BAG Fast Shipping</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/tote-bags-woven-canvastote-bag-little-miss-designs-custom-gifts-personalised-children-tote-bags-custom-bag-for-children-birthday-gifts-pets-bag-mr-men-tote-bag-fast-shipping-i2884174188.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>135 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FLOCK THREE Reusable Wet/Dry Waterproof Tote Bag Swimsuit Wet Clothes Laundry Bag Baby Diapers and Stroller Pouch</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/flock-three-reusable-wetdry-waterproof-tote-bag-swimsuit-wet-clothes-laundry-bag-baby-diapers-and-stroller-pouch-i1855852845.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$8.50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $0.43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>609 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tote Bag Handbag Cute Lunch Bag Goodie Bag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/tote-bag-handbag-cute-lunch-bag-goodie-bag-i3039282803.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>232 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Halloween MOJOYCE Harajuku Shoulder Bag Simple Shopping Bag Solid Color Satchel Bags Large Capacity Casual Zipper Soft Cloth for TeenagerChristmas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/halloween-mojoyce-harajuku-shoulder-bag-simple-shopping-bag-solid-color-satchel-bags-large-capacity-casual-zipper-soft-cloth-for-teenagerchristmas-i3184579153.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$7.45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 61%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shoulder Cotton Canvas Bag Tote bag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/shoulder-cotton-canvas-bag-tote-bag-i2655897514.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>93 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>169 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TINYAT Women's Summer Canvas Tote Bags Beach Shopping Bag Casual Cotton Handbag for Vacation - Stylish Beach Accessories</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/tinyat-womens-summer-canvas-tote-bags-beach-shopping-bag-casual-cotton-handbag-for-vacation-stylish-beach-accessories-i3431820267.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Early Bird Saved $8.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Folding Hiking Backpack Packable Lightweight Travel Unisex Sports Bag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/folding-hiking-backpack-packable-lightweight-travel-unisex-sports-bag-i1315438822.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>127 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mini Tote Bag Lightweight Short Strap NAVY GREEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/mini-tote-bag-lightweight-short-strap-navy-green-i2856814043.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100% Authentic Original Brand F58292 City Zip Tote Signature Canvas Women Handbag Shopping Shoulder Bag, Commodity Brand Packaging Size: 29*27*14cm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/100-authentic-original-brand-f58292-city-zip-tote-signature-canvas-women-handbag-shopping-shoulder-bag-commodity-brand-packaging-size-292714cm-i3380976816.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$59.48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 24%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NEENCA Waterproof Nylon Gym Bags Outdoor Sports Yoga Training Handbag Men Women Fitness Travel Storage Crossbody Sport Swimming Bags</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/neenca-waterproof-nylon-gym-bags-outdoor-sports-yoga-training-handbag-men-women-fitness-travel-storage-crossbody-sport-swimming-bags-i3280177920.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$7.31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SG SELLER Double Side Use Canvas Bag teachers day gifts Ladies Handbags gift ideas Canvas Tote Bag Shopping Bag Reusable Travel Bag Reversible Canvas Bag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sg-seller-double-side-use-canvas-bag-teachers-day-gifts-ladies-handbags-gift-ideas-canvas-tote-bag-shopping-bag-reusable-travel-bag-reversible-canvas-bag-i2727062797.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$7.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>400 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PUNKSTAR Portable Reusable Foldable Shopping Eco Tote Grocery Bags Water resistant Duffle Large Capacity for Shopping Camp Travel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/punkstar-portable-reusable-foldable-shopping-eco-tote-grocery-bags-water-resistant-duffle-large-capacity-for-shopping-camp-travel-i3009544629.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_xD83D__xDD25_{SG Seller}Canvas Bag Gift bag Cute Cartoon Bear Peach Mini Girl Heart Tote</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sg-sellercanvas-bag-gift-bag-cute-cartoon-bear-peach-mini-girl-heart-tote-i2868555449.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Army Bag / Hiking Backpack | 45L Large Size Bag | Spine Protection Bag | NS Bag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/army-bag-hiking-backpack-45l-large-size-bag-spine-protection-bag-ns-bag-i2901072121.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$28.90</x:t>
+  </x:si>
+  <x:si>
+    <x:t>91 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HOME ELEC-Desk Side Vertical Laptop Stand,No Drill Laptop Desktop Mount,Hanging Laptop Holder for Desk Side,Clamp on Desk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/home-elec-desk-side-vertical-laptop-standno-drill-laptop-desktop-mounthanging-laptop-holder-for-desk-sideclamp-on-desk-i3108839101.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$15.73</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LouisWill belt for women Belt Women's Leather Belt Ladies Skinny Belt Women's All-Match Belt Fashion Casual Thin Belt Waist Belt with Zinc Alloy Buckle for Jeans Pants ladies belt Women Belts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/louiswill-belt-for-women-belt-womens-leather-belt-ladies-skinny-belt-womens-all-match-belt-fashion-casual-thin-belt-waist-belt-with-zinc-alloy-buckle-for-jeans-pants-ladies-belt-women-belts-i2446854704.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 74%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>889 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LouisWill Women Belts Fashion Thin Belts Double Sided Use Elegant Thin Belt Gold Metal Hook Buckle Adjustable Girls Ladies Long Straps Waistbands Dress Coat Alloy Buckle Letter Buckle Gold Decorations</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/louiswill-women-belts-fashion-thin-belts-double-sided-use-elegant-thin-belt-gold-metal-hook-buckle-adjustable-girls-ladies-long-straps-waistbands-dress-coat-alloy-buckle-letter-buckle-gold-decorations-i2977220426.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$3.72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>61 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LouisWill Women Belts Fashion Thin Belts Elegant Thin Belt Gold Metal Hook Buckle Adjustable Girls Ladies Long Straps Waistbands Dress Coat Alloy Buckle Gold Decorations</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/louiswill-women-belts-fashion-thin-belts-elegant-thin-belt-gold-metal-hook-buckle-adjustable-girls-ladies-long-straps-waistbands-dress-coat-alloy-buckle-gold-decorations-i2884895817.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2.76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LouisWill Women Belts Waist Belt Ladies Casual Waistband Alloy Pin Buckle Belts PU Leather Belts Women’s Waist Belt Adjustable Length Dress Belt Vintage Jeans Belt for Women Girls</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/louiswill-women-belts-waist-belt-ladies-casual-waistbandalloy-pin-buckle-belts-pu-leather-belts-womens-waist-belt-adjustable-length-dress-belt-vintage-jeans-belt-for-women-girls-i2446741928.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$6.15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LouisWill Women's Belt Leather Belt Ladies Skinny Belt Women's All-Match Belt Fashion Casual Thin Belt Waist Belt with Zinc Alloy Buckle for Jeans Pants Gold Decorations Leisure Belt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/louiswill-womens-belt-leather-belt-ladies-skinny-belt-womens-all-match-belt-fashion-casual-thin-belt-waist-belt-with-zinc-alloy-buckle-for-jeans-pants-gold-decorations-leisure-belt-i3378097196.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4.40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LouisWill Women Belts Double Pearl Belts Casual Thin Belt Female Retro Black Red PU Leather Belt Dress Skirt Waist Elegant Pearl Leather Belts Elastic Thin Belts Ladies Designer Waistband</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/louiswill-women-belts-double-pearl-belts-casual-thin-belt-female-retro-black-red-pu-leather-belt-dress-skirt-waist-elegant-pearl-leather-belts-elastic-thin-belts-ladies-designer-waistband-i2446928351.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2.49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LouisWill Women Belts Fashion Double Sided Use Leather Belt Elegant Golden Square Buckle Design Adjustable Girls Ladies Long Straps Waistbands Dress Coat Alloy Buckle Letter Buckle Gold Decorations</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/louiswill-women-belts-fashion-double-sided-use-leather-belt-elegant-golden-square-buckle-design-adjustable-girls-ladies-long-straps-waistbands-dress-coat-alloy-buckle-letter-buckle-gold-decorations-i3071228317.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$6.82</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(FOREVER PREMIUM) Men Women Belt Wide Mesh Elastic</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/forever-premium-men-women-belt-wide-mesh-elastic-i2936564600.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$3.95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HolidayQueen Thin Belt Woman Knotted Decoration with Sweater Dress Suit Waist Fashion All-match Coat Small Belt Free Shipping HQ0273</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/holidayqueen-thin-belt-woman-knotted-decoration-with-sweater-dress-suit-waist-fashion-all-match-coat-small-belt-free-shipping-hq0273-i1932534425.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 33%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[SG] TechFave Premium Aluminium Laptop Stand Adjustable/Foldable/Portable/Universal Fit For MacBook/Laptops</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/sg-techfave-premium-aluminium-laptop-stand-adjustablefoldableportableuniversal-fit-for-macbooklaptops-i1877519306.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>READ Korean Elegant Women Dress Pearl Belt Adjustable Metal Chain Belt Jewelry Decoration</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/read-korean-elegant-women-dress-pearl-belt-adjustable-metal-chain-belt-jewelry-decoration-i2365287111.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>74 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JARUSEAT MR04 Laptop Stand/Monitor Stand 3 Height Adjustable Monitor Stand Ergonomic Metal Monitor Riser Stand with Mesh Platform</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/jaruseat-mr04-laptop-standmonitor-stand-3-height-adjustable-monitor-stand-ergonomic-metal-monitor-riser-stand-with-mesh-platform-i3297944116.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 41%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ODOROKU 4 in 1 Adjustable Vertical Laptop Stand Holder Double Triple Vertical Laptop Stand Supports Laptops Tablet Black White Pink</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/odoroku-4-in-1-adjustable-vertical-laptop-stand-holder-double-triple-vertical-laptop-stand-supports-laptops-tablet-black-white-pink-i3301787758.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MATEYOYO Fashion Women Belts Retro Belt Elegant Slim Belt Cow Leather Belt Adjustable Girls Ladies Long Straps Waistbands Dress Coat Alloy Buckle Letter Buckle Leisure Belt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/mateyoyo-fashion-women-belts-retro-belt-elegant-slim-belt-cow-leather-belt-adjustable-girls-ladies-long-straps-waistbands-dress-coat-alloy-buckle-letter-buckle-leisure-belt-i3399757369.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COWATHER Reversible Rotated Leather Casual Belts for Men - 1.3" wide Genuine Leather Belts - Fashion Classic Dress Durable Belts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/cowather-reversible-rotated-leather-casual-belts-for-men-13-wide-genuine-leather-belts-fashion-classic-dress-durable-belts-i3269633227.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MATEYOYO Women Belts Fashion Double Sided Use Leather Belt Elegant Golden Square Buckle Design Adjustable Girls Ladies Long Straps Waistbands Dress Coat Alloy Buckle Letter Buckle Gold Decorations</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/mateyoyo-women-belts-fashion-double-sided-use-leather-belt-elegant-golden-square-buckle-design-adjustable-girls-ladies-long-straps-waistbands-dress-coat-alloy-buckle-letter-buckle-gold-decorations-i3071431055.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$6.92</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nillkin Bolster/Bolster Plus Portable Stand for Laptop, Tablet, iPad, Mobile phones</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/nillkin-bolsterbolster-plus-portable-stand-for-laptop-tablet-ipad-mobile-phones-i2046844781.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$12.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 13%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alienware X17R2 Aluminum Alloy Notebook Stand Gaming Laptop Heat Sink Riser Storage Foldable Height Adjustable Suspension Cooling Rack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/alienware-x17r2-aluminum-alloy-notebook-stand-gaming-laptop-heat-sink-riser-storage-foldable-height-adjustable-suspension-cooling-rack-i3427599296.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$15.54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Squirrey Bace Laptop Tablet Vertical Adjustable Docking Stand [ Holder, Multiple Slot, &amp;lt;14", Lightweight, Storage, Office, Workspace, Desk Accessory ]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/squirrey-bace-laptop-tablet-vertical-adjustable-docking-stand-holder-multiple-slot-14-lightweight-storage-office-workspace-desk-accessory-i3167430099.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$16.90</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Msvii Aluminum Alloy Notebook Stand Portable Foldable Support Bracket for Thin Gaming Laptop Tablet Heat Dissipation Desktop Bracket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/msvii-aluminum-alloy-notebook-stand-portable-foldable-support-bracket-for-thin-gaming-laptop-tablet-heat-dissipation-desktop-bracket-i3425021069.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$16.96</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $0.51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>360 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MC N86 Foldable Laptop Stand 360°Rotation Notebook Aluminum Alloy Holder Portable Laptop Bracket with Heat Dissipation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/mc-n86-foldable-laptop-stand-360rotation-notebook-aluminum-alloy-holder-portable-laptop-bracket-with-heat-dissipation-i3050925866.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$48.90</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $2.45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Plus size Oxhide Full Grain Leather Belt -30mm /3cm - Casual Mens Belt- Belt with Jean Black /Brown/Tan-C21 HPOX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/plus-size-oxhide-full-grain-leather-belt-30mm-3cm-casual-mens-belt-belt-with-jean-black-browntan-c21-hpox-i535658956.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$20.61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $1.03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>438 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/squirrey-bace-laptop-tablet-vertical-adjustable-docking-stand-holder-multiple-slot-14-lightweight-storage-office-workspace-desk-accessory-i3167351833.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Belt Women - Belt Women Leather - Plus Size Available - Women belt in Full Grain Leather - Ladies Leather Belt - Oxhide -HPOX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/belt-women-belt-women-leather-plus-size-available-women-belt-in-full-grain-leather-ladies-leather-belt-oxhide-hpox-i324708237.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$17.10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $0.86</x:t>
+  </x:si>
+  <x:si>
+    <x:t>170 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Belt Women - Women Leather Designer Belt - Plus Size Available - Gold Buckle Women belt in Full Grain Leather - Designer Ladies Leather Belt in Black Color - Oxhide HPOX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/belt-women-women-leather-designer-belt-plus-size-available-gold-buckle-women-belt-in-full-grain-leather-designer-ladies-leather-belt-in-black-color-oxhide-hpox-i2466307185.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$26.91</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $1.35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mens Automatic Leather Belt - Full Grain Leather Ratchet Belt - Men Leather Belt with Auto Lock Buckle - TRACK BELT - Belt without hole - ABB5C Oxhide</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/mens-automatic-leather-belt-full-grain-leather-ratchet-belt-men-leather-belt-with-auto-lock-buckle-track-belt-belt-without-hole-abb5c-oxhide-i596924490.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$35.91</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $1.80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>38 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ULTi AURA RGB Vesa Laptop Holder | C74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/ulti-aura-rgb-vesa-laptop-holder-c74-i3135491502.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>POUT EYES 3 LIFT- A Height Adjustable Aluminum Standing Laptop Riser For 10 to 17inch</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/pout-eyes-3-lift-a-height-adjustable-aluminum-standing-laptop-riser-for-10-to-17inch-i2632179981.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$112.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EverDesk Adjustable Laptop Stand - 5 height, Lightweight, Foldable, Portable with Non-Slip Rubber Base</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/everdesk-adjustable-laptop-stand-5-height-lightweight-foldable-portable-with-non-slip-rubber-base-i265418388.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Voucher save 26%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>359 sold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ULTI Laptop Mount Tray Desk-ACC02 BLACK (Brought to you by Global Cybermind)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/ulti-laptop-mount-tray-desk-acc02-black-brought-to-you-by-global-cybermind-i2771177851.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$29.90</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LORDWEY New Gold Elevation Angle 20.58 ° Adjustable Aluminum With Expansion Base Laptop Stand</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/lordwey-new-gold-elevation-angle-2058-adjustable-aluminum-with-expansion-base-laptop-stand-i3381214932.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$59.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coin save $2.95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Banrique PC stand [supervised by physical therapist] Foldable, 6-level adjustable, lightweight design, heat dissipating, made of aluminum alloy (silver)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/banrique-pc-stand-supervised-by-physical-therapist-foldable-6-level-adjustable-lightweight-design-heat-dissipating-made-of-aluminum-alloy-silver-i3259583655.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$33.56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hobinavi laptop stand, foldable, compact, thermal runaway prevention, 7-step angle adjustment nts001-gy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/hobinavi-laptop-stand-foldable-compact-thermal-runaway-prevention-7-step-angle-adjustment-nts001-gy-i3259667333.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$44.97</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CM ERGO AIR SLIM NOTEBOOK STAND</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/cm-ergo-air-slim-notebook-stand-i2262389361.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Belmond Laptop Stand Vertical Aluminum Alloy Material [PC Sukkiri-kun] PC Stand 2 Units Storage Width Adjustable Clamshell Tablet MacBook Pro Air/Mac mini/iPad B091401 Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/belmond-laptop-stand-vertical-aluminum-alloy-material-pc-sukkiri-kun-pc-stand-2-units-storage-width-adjustable-clamshell-tablet-macbook-pro-airmac-miniipad-b091401-black-i3259656378.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$65.83</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOFT Cooling Stand Laptop stand with graphene Adhesive type vegan leather Reapplicable MacBook compatible Improved durability Heat dissipation Effect Instant setup</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/moft-cooling-stand-laptop-stand-with-graphene-adhesive-type-vegan-leather-reapplicable-macbook-compatible-improved-durability-heat-dissipation-effect-instant-setup-i3190467056.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$88.30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Baowor Desk Side Storage Clamp Desk Storage No drilling required 3-minute installation Desk Side Holder Laptop Stand Under Desk Storage Desk Side Rack Steel made Documents Laptop Tablet Phone Remote Control Stationery Cutlery Storage Organization ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/baowor-desk-side-storage-clamp-desk-storage-no-drilling-required-3-minute-installation-desk-side-holder-laptop-stand-under-desk-storage-desk-side-rack-steel-made-documents-laptop-tablet-phone-remote-control-stationery-cutlery-storage-organization-i3372862829.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$87.50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BIMI Bobo Style Braided Knotted Waist Belt Fashion Accessories Soft Boho Rope Chain Tie Waistband Solid Color Tassel Braided Waist Belt for Beginners</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/bimi-bobo-style-braided-knotted-waist-belt-fashion-accessories-soft-boho-rope-chain-tie-waistband-solid-color-tassel-braided-waist-belt-for-beginners-i3392769257.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>POLONE Elegant Women Accessories Sweater Decorative Wide Waist Belt Dress Strap Waistband Elastic Buckle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.lazada.sg/products/polone-elegant-women-accessories-sweater-decorative-wide-waist-belt-dress-strap-waistband-elastic-buckle-i3380917431.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.68</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -7938,4 +8994,2341 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F41"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>903</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
+        <x:v>904</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>905</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>906</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>907</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>908</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>909</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>910</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>911</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>912</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>913</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>914</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>747</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>915</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>916</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>917</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>918</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>919</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="0" t="s">
+        <x:v>315</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>316</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>920</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="0" t="s">
+        <x:v>921</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>922</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>923</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>924</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>925</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>926</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>927</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>469</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>576</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
+        <x:v>928</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>929</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>930</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0" t="s">
+        <x:v>921</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>931</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>932</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>933</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0" t="s">
+        <x:v>934</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>935</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>936</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>255</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>482</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0" t="s">
+        <x:v>937</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>938</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0" t="s">
+        <x:v>939</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>940</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>941</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>406</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>652</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>942</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>943</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>944</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0" t="s">
+        <x:v>945</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>946</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>947</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>948</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" s="0" t="s">
+        <x:v>949</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>950</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>951</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0" t="s">
+        <x:v>952</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>953</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>954</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>491</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0" t="s">
+        <x:v>955</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>956</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>957</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>911</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0" t="s">
+        <x:v>958</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>959</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>588</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>960</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0" t="s">
+        <x:v>961</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>962</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>963</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>964</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0" t="s">
+        <x:v>965</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>966</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>967</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>395</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>968</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" s="0" t="s">
+        <x:v>969</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>970</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>971</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>972</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
+        <x:v>973</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>974</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>975</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>976</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
+        <x:v>977</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>978</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>979</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>980</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
+        <x:v>981</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>982</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>983</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>410</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0" t="s">
+        <x:v>984</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>985</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>986</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>911</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" s="0" t="s">
+        <x:v>987</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>988</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>989</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" s="0" t="s">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>451</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>482</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" s="0" t="s">
+        <x:v>435</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>990</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>991</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" s="0" t="s">
+        <x:v>992</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>993</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>971</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>994</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="0" t="s">
+        <x:v>995</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>996</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>997</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>998</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0" t="s">
+        <x:v>999</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>1001</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>1002</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0" t="s">
+        <x:v>1003</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>1004</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>878</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="0" t="s">
+        <x:v>1005</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>1006</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>1007</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F37" s="0" t="s">
+        <x:v>1008</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="0" t="s">
+        <x:v>1009</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>1010</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="0" t="s">
+        <x:v>1011</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>1012</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>1013</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>1014</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" s="0" t="s">
+        <x:v>1015</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>1016</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>1017</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>1018</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" s="0" t="s">
+        <x:v>1019</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>1020</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>1021</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>469</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>652</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F41"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="0" t="s">
+        <x:v>1022</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>1023</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>1024</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>486</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
+        <x:v>1025</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>1026</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>1027</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>1028</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>1029</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>1030</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>1031</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>1032</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>1033</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>1034</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>1035</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>1036</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>1037</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>780</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>1038</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>1039</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>688</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>495</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>1040</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
+        <x:v>799</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>800</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>801</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>1041</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="0" t="s">
+        <x:v>1042</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>1043</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>1044</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>1045</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="0" t="s">
+        <x:v>1046</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>1047</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>473</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>1048</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>781</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>782</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>1049</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>1050</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
+        <x:v>1051</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>1052</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>1053</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>1054</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0" t="s">
+        <x:v>1055</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>1056</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>1057</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>901</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0" t="s">
+        <x:v>1058</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>1059</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>1060</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>1061</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0" t="s">
+        <x:v>872</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>873</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>874</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>438</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>499</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0" t="s">
+        <x:v>1062</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>1063</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>456</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>1064</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>822</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>823</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>824</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>825</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>826</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0" t="s">
+        <x:v>1065</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>1066</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>1067</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" s="0" t="s">
+        <x:v>1068</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>1069</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>786</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>747</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0" t="s">
+        <x:v>1070</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>1071</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>859</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>625</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0" t="s">
+        <x:v>1072</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>1073</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>1074</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>1075</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0" t="s">
+        <x:v>1076</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>1077</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>548</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>855</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>1078</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0" t="s">
+        <x:v>1079</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>1080</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>1081</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0" t="s">
+        <x:v>1082</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>1083</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>1084</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>1085</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>1086</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0" t="s">
+        <x:v>1087</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>1088</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>1089</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>1090</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" s="0" t="s">
+        <x:v>803</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>804</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>805</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>806</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>807</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
+        <x:v>1091</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>1092</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>1093</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>1094</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>951</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
+        <x:v>1095</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>1096</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>878</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>747</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>1097</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
+        <x:v>784</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>785</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>786</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>787</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>788</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0" t="s">
+        <x:v>879</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>880</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>881</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>882</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" s="0" t="s">
+        <x:v>763</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>764</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>765</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>766</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>1098</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" s="0" t="s">
+        <x:v>1099</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>1100</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>417</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>1101</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" s="0" t="s">
+        <x:v>842</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>843</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>815</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>844</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" s="0" t="s">
+        <x:v>1102</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>1103</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>770</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>771</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>1104</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="0" t="s">
+        <x:v>857</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>858</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>859</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0" t="s">
+        <x:v>1105</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>1106</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>456</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>395</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0" t="s">
+        <x:v>1107</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>1108</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>1109</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>1110</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="0" t="s">
+        <x:v>1111</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>1112</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>1113</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="0" t="s">
+        <x:v>1114</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>1115</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>1116</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>901</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>1117</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="0" t="s">
+        <x:v>1118</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>1119</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>539</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F39" s="0" t="s">
+        <x:v>736</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" s="0" t="s">
+        <x:v>1120</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>1121</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" s="0" t="s">
+        <x:v>1122</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>1123</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>1124</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>732</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>1125</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F41"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>1127</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>1128</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
+        <x:v>1129</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>1130</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>628</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>1131</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>1132</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>1133</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>1134</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>1135</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>1136</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>1137</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>1138</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>1139</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>331</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>1140</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>1141</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>1142</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>991</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
+        <x:v>1143</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>1144</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>1145</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>766</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="0" t="s">
+        <x:v>1146</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>1147</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>1148</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>801</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>591</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="0" t="s">
+        <x:v>1149</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>1150</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>1151</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>693</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>1152</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>1153</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>1154</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
+        <x:v>1155</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>1156</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>743</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>1157</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0" t="s">
+        <x:v>1158</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>1159</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>491</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0" t="s">
+        <x:v>1160</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>1161</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>1060</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>1162</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0" t="s">
+        <x:v>1163</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>1164</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>1165</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>283</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0" t="s">
+        <x:v>1166</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>1167</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>721</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>707</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>1168</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>1169</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>989</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>486</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0" t="s">
+        <x:v>1170</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>1171</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" s="0" t="s">
+        <x:v>1172</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>1173</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>1174</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>766</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0" t="s">
+        <x:v>1175</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>1176</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>1177</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>1178</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0" t="s">
+        <x:v>1179</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>1180</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>1181</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>998</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0" t="s">
+        <x:v>1182</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>1183</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>1184</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0" t="s">
+        <x:v>1185</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>1186</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>1187</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>1188</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>1189</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0" t="s">
+        <x:v>1190</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>1191</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>1192</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>1193</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0" t="s">
+        <x:v>1194</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>1195</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>1196</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>1197</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>1198</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" s="0" t="s">
+        <x:v>1182</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>1199</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>511</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>1178</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
+        <x:v>1200</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>1201</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>1202</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>1203</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>1204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
+        <x:v>1205</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>1206</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>1207</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>1208</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>1209</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
+        <x:v>1210</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>1211</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>1212</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>1213</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>1214</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0" t="s">
+        <x:v>1215</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>1216</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>810</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>811</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>911</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" s="0" t="s">
+        <x:v>1217</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>1218</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>1219</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" s="0" t="s">
+        <x:v>1220</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>1221</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>731</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>1222</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>1223</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" s="0" t="s">
+        <x:v>1224</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>1225</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>1226</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" s="0" t="s">
+        <x:v>1227</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>1228</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>1229</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>1230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="0" t="s">
+        <x:v>1231</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>1232</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>1233</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>1018</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0" t="s">
+        <x:v>1234</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>1235</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>1236</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>1018</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0" t="s">
+        <x:v>1237</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>1238</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>1229</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="0" t="s">
+        <x:v>1239</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>1240</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>1241</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>1018</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="0" t="s">
+        <x:v>1242</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>1243</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>1244</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>1018</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="0" t="s">
+        <x:v>1245</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>1246</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>1247</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>1018</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" s="0" t="s">
+        <x:v>1248</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>1249</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>1250</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>571</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" s="0" t="s">
+        <x:v>1251</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>1252</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>1253</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>603</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Final Result of Shopee
</commit_message>
<xml_diff>
--- a/Data/Products_Lazada.xlsx
+++ b/Data/Products_Lazada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e110b5800b3f798d/南洋理工/MSBA-T3/AN6817 - ROBOTIC PROCESS AUTOMATION (RPA) FOR ANALYTICS/Group Project/TeamProject/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e110b5800b3f798d/Documents/UiPath/AN6817-TeamProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_A5AE680E52BCE59F1BC5729A91226002E16658FE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01F338EA-63DB-4BF4-9D87-60ABEC9B17C6}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_A5AE680E52BCE59F1BC5729A91226002E16658FE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88E2A230-0126-4C74-BA73-EA4B3058A08B}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="285" windowWidth="29040" windowHeight="16035" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5550" yWindow="4490" windowWidth="19200" windowHeight="11710" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoes-for-men" sheetId="5" r:id="rId1"/>
@@ -5777,10 +5777,13 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>